<commit_message>
Retention of Escolars no contesten. Added escolars_no_contesten sheet to the final report.Modifies fig4
</commit_message>
<xml_diff>
--- a/Metaarxius/Esquema_taula8.xlsx
+++ b/Metaarxius/Esquema_taula8.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Casuístiques segons "resultat de verificació" eligibles de seguiment (a)</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>No contesta (sense "escolars")</t>
+  </si>
+  <si>
+    <t>No contesta ("escolar")</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,21 +529,28 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>